<commit_message>
Fix to list and added FI on date
</commit_message>
<xml_diff>
--- a/app/config/tables/ParmaComsup/Forms/ParmaComsup/ParmaComsup.xlsx
+++ b/app/config/tables/ParmaComsup/Forms/ParmaComsup/ParmaComsup.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FD0A0F-E250-4F95-BBBC-10C3EF447631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04539E81-9595-4985-A949-517991F4068E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="136">
   <si>
     <t>setting_name</t>
   </si>
@@ -218,9 +218,6 @@
     <t>dapamans</t>
   </si>
   <si>
-    <t>data('dapamans') != null</t>
-  </si>
-  <si>
     <t>IDPAMA</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>dacomsupns</t>
   </si>
   <si>
-    <t>data('dacomsupns') != null</t>
-  </si>
-  <si>
     <t>IDCOMSUP</t>
   </si>
   <si>
@@ -435,6 +429,18 @@
   </si>
   <si>
     <t>Par Mamar:</t>
+  </si>
+  <si>
+    <t>data('dapamans') == "D:1,M:1,Y:1955"</t>
+  </si>
+  <si>
+    <t>data('dacomsupns')  == "D:1,M:1,Y:1955"</t>
+  </si>
+  <si>
+    <t>data('dacomsupns')  == "D:NS,M:NS,Y:NS"  || data('DACOMSUP')  == "D:NS,M:NS,Y:NS"</t>
+  </si>
+  <si>
+    <t>data('dapamans') == "D:NS,M:NS,Y:NS" || data('DAPAMA') == "D:NS,M:NS,Y:NS"</t>
   </si>
 </sst>
 </file>
@@ -938,7 +944,7 @@
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -952,12 +958,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787AB6FC-E5B2-448F-8A60-6571052C1548}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,13 +1011,13 @@
         <v>22</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>49</v>
@@ -1019,7 +1025,7 @@
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1027,10 +1033,10 @@
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1038,10 +1044,10 @@
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1049,10 +1055,10 @@
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1060,10 +1066,10 @@
         <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1071,10 +1077,10 @@
         <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1082,10 +1088,10 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1093,10 +1099,10 @@
         <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1104,10 +1110,10 @@
         <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1115,10 +1121,10 @@
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1126,15 +1132,15 @@
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1142,12 +1148,12 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1155,10 +1161,10 @@
         <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -1166,16 +1172,16 @@
         <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
         <v>66</v>
-      </c>
-      <c r="H17" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -1183,7 +1189,7 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -1200,7 +1206,7 @@
         <v>56</v>
       </c>
       <c r="J19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K19" t="s">
         <v>57</v>
@@ -1228,7 +1234,7 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -1236,13 +1242,13 @@
         <v>38</v>
       </c>
       <c r="F22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" t="s">
         <v>62</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>63</v>
-      </c>
-      <c r="H22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
@@ -1253,7 +1259,7 @@
         <v>54</v>
       </c>
       <c r="I23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
@@ -1263,12 +1269,21 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>91</v>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
@@ -1278,88 +1293,58 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" t="s">
-        <v>132</v>
-      </c>
-      <c r="H30" t="s">
-        <v>132</v>
+      <c r="B30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" t="s">
-        <v>71</v>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>30</v>
-      </c>
-      <c r="F33" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="H33" t="s">
-        <v>75</v>
-      </c>
-      <c r="J33" t="s">
-        <v>96</v>
-      </c>
-      <c r="K33" t="s">
-        <v>76</v>
-      </c>
-      <c r="L33" t="s">
-        <v>77</v>
-      </c>
-      <c r="M33" t="b">
-        <v>0</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="G34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -1367,51 +1352,120 @@
         <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G36" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H36" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="J36" t="s">
+        <v>94</v>
+      </c>
+      <c r="K36" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" t="s">
+        <v>76</v>
+      </c>
+      <c r="M36" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="E37" t="s">
+        <v>59</v>
       </c>
       <c r="F37" t="s">
-        <v>73</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>41</v>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" t="s">
+        <v>78</v>
+      </c>
+      <c r="G39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>91</v>
+      <c r="D40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1427,7 +1481,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,14 +1508,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -1469,7 +1523,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" t="str">
         <f>"2"</f>
@@ -1484,7 +1538,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" t="str">
         <f>"3"</f>
@@ -1499,17 +1553,17 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" t="str">
         <f>"9"</f>
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,14 +1575,26 @@
         <v>D:NS,M:NS,Y:NS</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"D:1,M:1,Y:1955"</f>
+        <v>D:1,M:1,Y:1955</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1843,26 +1909,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +2020,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1965,7 +2031,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
@@ -1976,7 +2042,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -1987,7 +2053,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -1998,7 +2064,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
@@ -2009,7 +2075,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -2020,10 +2086,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -2031,10 +2097,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
         <v>106</v>
-      </c>
-      <c r="B9" t="s">
-        <v>108</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2042,7 +2108,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
         <v>38</v>
@@ -2053,7 +2119,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -2064,7 +2130,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
@@ -2075,7 +2141,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
@@ -2086,7 +2152,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -2097,7 +2163,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -2108,7 +2174,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -2141,7 +2207,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
@@ -2152,7 +2218,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
@@ -2163,7 +2229,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
         <v>38</v>
@@ -2174,7 +2240,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
         <v>38</v>
@@ -2185,7 +2251,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
@@ -2196,7 +2262,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Master -> LMP cleaning branch2
</commit_message>
<xml_diff>
--- a/app/config/tables/ParmaComsup/Forms/ParmaComsup/ParmaComsup.xlsx
+++ b/app/config/tables/ParmaComsup/Forms/ParmaComsup/ParmaComsup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afisker\Documents\tablet\DataClean-ParmaComsup\app\config\tables\ParmaComsup\Forms\ParmaComsup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05B7BB3-24C8-485F-89C5-9FA26B67D681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F30CDD3-5A58-4D23-9A8F-C4DFAEC62A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="114">
   <si>
     <t>setting_name</t>
   </si>
@@ -344,9 +344,6 @@
     <t>Codigo de assistente na data {{data.CONT}}</t>
   </si>
   <si>
-    <t>Quali informacao sobre data ult mens?</t>
-  </si>
-  <si>
     <t>"00"</t>
   </si>
   <si>
@@ -369,6 +366,21 @@
   </si>
   <si>
     <t>ParmaComsup</t>
+  </si>
+  <si>
+    <t>Qual e informacao sobre data ult mens?</t>
+  </si>
+  <si>
+    <t>Data de visita: &lt;b&gt;{{data.CONT}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>NOVIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numero de visita: &lt;b&gt;{{data.NOVIS}}&lt;/b&gt; </t>
+  </si>
+  <si>
+    <t>Qual e informacao sobre data do ult mens?</t>
   </si>
 </sst>
 </file>
@@ -659,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,7 +710,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -714,7 +726,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -722,10 +734,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -774,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="H2" sqref="A2:H25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -845,7 +857,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
         <v>81</v>
@@ -856,7 +868,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
         <v>80</v>
@@ -867,7 +879,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
         <v>79</v>
@@ -878,7 +890,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
         <v>78</v>
@@ -889,7 +901,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
         <v>82</v>
@@ -900,13 +912,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -930,7 +942,7 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -940,89 +952,111 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
         <v>76</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>96</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>75</v>
       </c>
-      <c r="G13" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>105</v>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D17" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
         <v>98</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F19" t="s">
         <v>99</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G19" t="s">
         <v>100</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H19" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" t="s">
-        <v>44</v>
+      <c r="B23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1301,10 +1335,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1406,10 +1440,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1436,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="A2:C18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1539,7 +1573,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -1644,6 +1678,17 @@
         <v>39</v>
       </c>
       <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>